<commit_message>
Behavior translation. Single Senior already modelled
</commit_message>
<xml_diff>
--- a/res/recipetimeconverter.xlsx
+++ b/res/recipetimeconverter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jevora\repositories\tafat\tafat\SmartCities\model\electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jevora\repositories\tafat\tafat\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="25">
   <si>
     <t>Lighting.class</t>
   </si>
@@ -85,6 +85,21 @@
   <si>
     <t>SingleSenior #1</t>
   </si>
+  <si>
+    <t>SingleSenior #2</t>
+  </si>
+  <si>
+    <t>Dishwasher.class</t>
+  </si>
+  <si>
+    <t>SingleSenior #3</t>
+  </si>
+  <si>
+    <t>SingleSenior #4</t>
+  </si>
+  <si>
+    <t>Microwave.class</t>
+  </si>
 </sst>
 </file>
 
@@ -122,10 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,17 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -473,11 +488,11 @@
         <v>90</v>
       </c>
       <c r="F3" s="1">
-        <f>((B3+360)/60)/24</f>
+        <f t="shared" ref="F3:F14" si="0">((B3+360)/60)/24</f>
         <v>0.29166666666666669</v>
       </c>
       <c r="G3" s="1">
-        <f>((C3+360)/60)/24</f>
+        <f t="shared" ref="G3:G14" si="1">((C3+360)/60)/24</f>
         <v>0.29166666666666669</v>
       </c>
       <c r="H3" s="1">
@@ -489,11 +504,11 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <f>((E3-D3)/2)+D3</f>
+        <f t="shared" ref="J3:J14" si="2">((E3-D3)/2)+D3</f>
         <v>90</v>
       </c>
       <c r="K3" s="2">
-        <f>E3-J3</f>
+        <f t="shared" ref="K3:K14" si="3">E3-J3</f>
         <v>0</v>
       </c>
     </row>
@@ -514,27 +529,27 @@
         <v>2</v>
       </c>
       <c r="F4" s="1">
-        <f>((B4+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.2986111111111111</v>
       </c>
       <c r="G4" s="1">
-        <f>((C4+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.30555555555555552</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H9" si="0">(((G4-F4)/2)+F4)</f>
+        <f t="shared" ref="H4:H9" si="4">(((G4-F4)/2)+F4)</f>
         <v>0.30208333333333331</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I9" si="1">H4-F4</f>
+        <f t="shared" ref="I4:I9" si="5">H4-F4</f>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="J4" s="2">
-        <f>((E4-D4)/2)+D4</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K4" s="2">
-        <f>E4-J4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -555,27 +570,27 @@
         <v>30</v>
       </c>
       <c r="F5" s="1">
-        <f>((B5+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.31944444444444448</v>
       </c>
       <c r="G5" s="1">
-        <f>((C5+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.3263888888888889</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.32291666666666669</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="J5" s="2">
-        <f>((E5-D5)/2)+D5</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="K5" s="2">
-        <f>E5-J5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -596,27 +611,27 @@
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f>((B6+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G6" s="1">
-        <f>((C6+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.8125</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.80208333333333326</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J6" s="2">
-        <f>((E6-D6)/2)+D6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f>E6-J6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -637,27 +652,27 @@
         <v>30</v>
       </c>
       <c r="F7" s="1">
-        <f>((B7+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.8125</v>
       </c>
       <c r="G7" s="1">
-        <f>((C7+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.81944444444444453</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.81597222222222232</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="J7" s="2">
-        <f>((E7-D7)/2)+D7</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="K7" s="2">
-        <f>E7-J7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -678,27 +693,27 @@
         <v>60</v>
       </c>
       <c r="F8" s="1">
-        <f>((B8+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.84027777777777779</v>
       </c>
       <c r="G8" s="1">
-        <f>((C8+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.84722222222222221</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.84375</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="J8" s="2">
-        <f>((E8-D8)/2)+D8</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="K8" s="2">
-        <f>E8-J8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -719,27 +734,27 @@
         <v>15</v>
       </c>
       <c r="F9" s="1">
-        <f>((B9+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
       <c r="G9" s="1">
-        <f>((C9+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.89583333333333337</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.89236111111111116</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="J9" s="2">
-        <f>((E9-D9)/2)+D9</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="K9" s="2">
-        <f>E9-J9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -760,11 +775,11 @@
         <v>90</v>
       </c>
       <c r="F10" s="1">
-        <f>((B10+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.90625</v>
       </c>
       <c r="G10" s="1">
-        <f>((C10+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.91319444444444453</v>
       </c>
       <c r="H10" s="1">
@@ -776,11 +791,11 @@
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="J10" s="2">
-        <f>((E10-D10)/2)+D10</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="K10" s="2">
-        <f>E10-J10</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -801,27 +816,27 @@
         <v>120</v>
       </c>
       <c r="F11" s="1">
-        <f>((B11+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.95486111111111116</v>
       </c>
       <c r="G11" s="1">
-        <f>((C11+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.96180555555555547</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H14" si="2">(((G11-F11)/2)+F11)</f>
+        <f t="shared" ref="H11:H14" si="6">(((G11-F11)/2)+F11)</f>
         <v>0.95833333333333326</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ref="I11:I14" si="3">H11-F11</f>
+        <f t="shared" ref="I11:I14" si="7">H11-F11</f>
         <v>3.4722222222220989E-3</v>
       </c>
       <c r="J11" s="2">
-        <f>((E11-D11)/2)+D11</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="K11" s="2">
-        <f>E11-J11</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
     </row>
@@ -842,27 +857,27 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <f>((B12+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.95833333333333337</v>
       </c>
       <c r="G12" s="1">
-        <f>((C12+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>1.0416666666666667</v>
       </c>
       <c r="H12" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="7"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="J12" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="K12" s="2">
         <f t="shared" si="3"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="J12" s="2">
-        <f>((E12-D12)/2)+D12</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <f>E12-J12</f>
         <v>0</v>
       </c>
     </row>
@@ -883,27 +898,27 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <f>((B13+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G13" s="1">
-        <f>((C13+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" si="6"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="7"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="J13" s="2">
         <f t="shared" si="2"/>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
         <f t="shared" si="3"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="J13" s="2">
-        <f>((E13-D13)/2)+D13</f>
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <f>E13-J13</f>
         <v>0</v>
       </c>
     </row>
@@ -924,27 +939,27 @@
         <v>5</v>
       </c>
       <c r="F14" s="1">
-        <f>((B14+360)/60)/24</f>
+        <f t="shared" si="0"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G14" s="1">
-        <f>((C14+360)/60)/24</f>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
       <c r="H14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="7"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="J14" s="2">
         <f t="shared" si="2"/>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" si="3"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="J14" s="2">
-        <f>((E14-D14)/2)+D14</f>
-        <v>4</v>
-      </c>
-      <c r="K14" s="2">
-        <f>E14-J14</f>
         <v>1</v>
       </c>
     </row>
@@ -974,27 +989,27 @@
         <v>60</v>
       </c>
       <c r="F16" s="1">
-        <f>((B16+360)/60)/24</f>
+        <f t="shared" ref="F16:F26" si="8">((B16+360)/60)/24</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="G16" s="1">
-        <f>((C16+360)/60)/24</f>
+        <f t="shared" ref="G16:G26" si="9">((C16+360)/60)/24</f>
         <v>0.34027777777777773</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" ref="H16" si="4">(((G16-F16)/2)+F16)</f>
+        <f t="shared" ref="H16" si="10">(((G16-F16)/2)+F16)</f>
         <v>0.33680555555555552</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" ref="I16" si="5">H16-F16</f>
+        <f t="shared" ref="I16" si="11">H16-F16</f>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="J16" s="2">
-        <f>((E16-D16)/2)+D16</f>
+        <f t="shared" ref="J16:J26" si="12">((E16-D16)/2)+D16</f>
         <v>52.5</v>
       </c>
       <c r="K16" s="2">
-        <f>E16-J16</f>
+        <f t="shared" ref="K16:K26" si="13">E16-J16</f>
         <v>7.5</v>
       </c>
     </row>
@@ -1015,27 +1030,27 @@
         <v>5</v>
       </c>
       <c r="F17" s="1">
-        <f>((B17+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.34027777777777773</v>
       </c>
       <c r="G17" s="1">
-        <f>((C17+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.34375</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17:H26" si="6">(((G17-F17)/2)+F17)</f>
+        <f t="shared" ref="H17:H26" si="14">(((G17-F17)/2)+F17)</f>
         <v>0.34201388888888884</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="I17:I26" si="7">H17-F17</f>
+        <f t="shared" ref="I17:I26" si="15">H17-F17</f>
         <v>1.7361111111111049E-3</v>
       </c>
       <c r="J17" s="2">
-        <f>((E17-D17)/2)+D17</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K17" s="2">
-        <f>E17-J17</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -1056,27 +1071,27 @@
         <v>30</v>
       </c>
       <c r="F18" s="1">
-        <f>((B18+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.34027777777777773</v>
       </c>
       <c r="G18" s="1">
-        <f>((C18+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.34375</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.34201388888888884</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>1.7361111111111049E-3</v>
       </c>
       <c r="J18" s="2">
-        <f>((E18-D18)/2)+D18</f>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
       <c r="K18" s="2">
-        <f>E18-J18</f>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
     </row>
@@ -1097,27 +1112,27 @@
         <v>-1</v>
       </c>
       <c r="F19" s="1">
-        <f>((B19+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
       <c r="G19" s="1">
-        <f>((C19+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.76388888888888884</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.75694444444444442</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J19" s="2">
-        <f>((E19-D19)/2)+D19</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <f>E19-J19</f>
+        <f t="shared" si="13"/>
         <v>-1</v>
       </c>
     </row>
@@ -1138,27 +1153,27 @@
         <v>30</v>
       </c>
       <c r="F20" s="1">
-        <f>((B20+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.77083333333333337</v>
       </c>
       <c r="G20" s="1">
-        <f>((C20+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.78125</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J20" s="2">
-        <f>((E20-D20)/2)+D20</f>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="K20" s="2">
-        <f>E20-J20</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1179,27 +1194,27 @@
         <v>30</v>
       </c>
       <c r="F21" s="1">
-        <f>((B21+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G21" s="1">
-        <f>((C21+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.8125</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="J21" s="2">
-        <f>((E21-D21)/2)+D21</f>
+        <f t="shared" si="12"/>
         <v>27.5</v>
       </c>
       <c r="K21" s="2">
-        <f>E21-J21</f>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1220,27 +1235,27 @@
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <f>((B22+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G22" s="1">
-        <f>((C22+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.8125</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="J22" s="2">
-        <f>((E22-D22)/2)+D22</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="K22" s="2">
-        <f>E22-J22</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -1261,27 +1276,27 @@
         <v>30</v>
       </c>
       <c r="F23" s="1">
-        <f>((B23+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G23" s="1">
-        <f>((C23+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.80555555555555547</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.79861111111111105</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J23" s="2">
-        <f>((E23-D23)/2)+D23</f>
+        <f t="shared" si="12"/>
         <v>27.5</v>
       </c>
       <c r="K23" s="2">
-        <f>E23-J23</f>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1302,27 +1317,27 @@
         <v>120</v>
       </c>
       <c r="F24" s="1">
-        <f>((B24+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G24" s="1">
-        <f>((C24+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.875</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="J24" s="2">
-        <f>((E24-D24)/2)+D24</f>
+        <f t="shared" si="12"/>
         <v>105</v>
       </c>
       <c r="K24" s="2">
-        <f>E24-J24</f>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
     </row>
@@ -1343,27 +1358,27 @@
         <v>120</v>
       </c>
       <c r="F25" s="1">
-        <f>((B25+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G25" s="1">
-        <f>((C25+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.875</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="J25" s="2">
-        <f>((E25-D25)/2)+D25</f>
+        <f t="shared" si="12"/>
         <v>105</v>
       </c>
       <c r="K25" s="2">
-        <f>E25-J25</f>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
     </row>
@@ -1384,27 +1399,27 @@
         <v>-1</v>
       </c>
       <c r="F26" s="1">
-        <f>((B26+360)/60)/24</f>
+        <f t="shared" si="8"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="G26" s="1">
-        <f>((C26+360)/60)/24</f>
+        <f t="shared" si="9"/>
         <v>0.95833333333333337</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>0.9375</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="J26" s="2">
-        <f>((E26-D26)/2)+D26</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K26" s="2">
-        <f>E26-J26</f>
+        <f t="shared" si="13"/>
         <v>-1</v>
       </c>
     </row>
@@ -1434,27 +1449,27 @@
         <v>75</v>
       </c>
       <c r="F28" s="1">
-        <f>((B28+360)/60)/24</f>
+        <f t="shared" ref="F28:G35" si="16">((B28+360)/60)/24</f>
         <v>0.3125</v>
       </c>
       <c r="G28" s="1">
-        <f>((C28+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" ref="H28" si="8">(((G28-F28)/2)+F28)</f>
+        <f t="shared" ref="H28" si="17">(((G28-F28)/2)+F28)</f>
         <v>0.32291666666666663</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" ref="I28" si="9">H28-F28</f>
+        <f t="shared" ref="I28" si="18">H28-F28</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J28" s="2">
-        <f>((E28-D28)/2)+D28</f>
+        <f t="shared" ref="J28:J35" si="19">((E28-D28)/2)+D28</f>
         <v>67.5</v>
       </c>
       <c r="K28" s="2">
-        <f>E28-J28</f>
+        <f t="shared" ref="K28:K35" si="20">E28-J28</f>
         <v>7.5</v>
       </c>
     </row>
@@ -1475,27 +1490,27 @@
         <v>30</v>
       </c>
       <c r="F29" s="1">
-        <f>((B29+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.31597222222222221</v>
       </c>
       <c r="G29" s="1">
-        <f>((C29+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.33680555555555558</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" ref="H29:H35" si="10">(((G29-F29)/2)+F29)</f>
+        <f t="shared" ref="H29:H35" si="21">(((G29-F29)/2)+F29)</f>
         <v>0.3263888888888889</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" ref="I29:I35" si="11">H29-F29</f>
+        <f t="shared" ref="I29:I35" si="22">H29-F29</f>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="J29" s="2">
-        <f>((E29-D29)/2)+D29</f>
+        <f t="shared" si="19"/>
         <v>25</v>
       </c>
       <c r="K29" s="2">
-        <f>E29-J29</f>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
     </row>
@@ -1516,27 +1531,27 @@
         <v>-1</v>
       </c>
       <c r="F30" s="1">
-        <f>((B30+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G30" s="1">
-        <f>((C30+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.80555555555555547</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.79861111111111105</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J30" s="2">
-        <f>((E30-D30)/2)+D30</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K30" s="2">
-        <f>E30-J30</f>
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
@@ -1557,27 +1572,27 @@
         <v>-1</v>
       </c>
       <c r="F31" s="1">
-        <f>((B31+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.79861111111111116</v>
       </c>
       <c r="G31" s="1">
-        <f>((C31+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.8125</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.80555555555555558</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J31" s="2">
-        <f>((E31-D31)/2)+D31</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K31" s="2">
-        <f>E31-J31</f>
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
@@ -1598,27 +1613,27 @@
         <v>-1</v>
       </c>
       <c r="F32" s="1">
-        <f>((B32+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G32" s="1">
-        <f>((C32+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.875</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.83333333333333326</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="J32" s="2">
-        <f>((E32-D32)/2)+D32</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K32" s="2">
-        <f>E32-J32</f>
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
@@ -1639,27 +1654,27 @@
         <v>10</v>
       </c>
       <c r="F33" s="1">
-        <f>((B33+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.85416666666666663</v>
       </c>
       <c r="G33" s="1">
-        <f>((C33+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.875</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.86458333333333326</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J33" s="2">
-        <f>((E33-D33)/2)+D33</f>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="K33" s="2">
-        <f>E33-J33</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
@@ -1680,27 +1695,27 @@
         <v>-1</v>
       </c>
       <c r="F34" s="1">
-        <f>((B34+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.88194444444444453</v>
       </c>
       <c r="G34" s="1">
-        <f>((C34+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.89583333333333337</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.88888888888888895</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J34" s="2">
-        <f>((E34-D34)/2)+D34</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K34" s="2">
-        <f>E34-J34</f>
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
@@ -1721,27 +1736,27 @@
         <v>-1</v>
       </c>
       <c r="F35" s="1">
-        <f>((B35+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>0.9375</v>
       </c>
       <c r="G35" s="1">
-        <f>((C35+360)/60)/24</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="21"/>
         <v>0.96875</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>3.125E-2</v>
       </c>
       <c r="J35" s="2">
-        <f>((E35-D35)/2)+D35</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K35" s="2">
-        <f>E35-J35</f>
+        <f t="shared" si="20"/>
         <v>-1</v>
       </c>
     </row>
@@ -1771,27 +1786,27 @@
         <v>60</v>
       </c>
       <c r="F37" s="1">
-        <f>((B37+360)/60)/24</f>
+        <f t="shared" ref="F37:F45" si="23">((B37+360)/60)/24</f>
         <v>0.32291666666666669</v>
       </c>
       <c r="G37" s="1">
-        <f>((C37+360)/60)/24</f>
+        <f t="shared" ref="G37:G45" si="24">((C37+360)/60)/24</f>
         <v>0.32291666666666669</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" ref="H37" si="12">(((G37-F37)/2)+F37)</f>
+        <f t="shared" ref="H37" si="25">(((G37-F37)/2)+F37)</f>
         <v>0.32291666666666669</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" ref="I37" si="13">H37-F37</f>
+        <f t="shared" ref="I37" si="26">H37-F37</f>
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <f>((E37-D37)/2)+D37</f>
+        <f t="shared" ref="J37:J45" si="27">((E37-D37)/2)+D37</f>
         <v>52.5</v>
       </c>
       <c r="K37" s="2">
-        <f>E37-J37</f>
+        <f t="shared" ref="K37:K45" si="28">E37-J37</f>
         <v>7.5</v>
       </c>
     </row>
@@ -1812,27 +1827,27 @@
         <v>5</v>
       </c>
       <c r="F38" s="1">
-        <f>((B38+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G38" s="1">
-        <f>((C38+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.33680555555555558</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" ref="H38:H45" si="14">(((G38-F38)/2)+F38)</f>
+        <f t="shared" ref="H38:H45" si="29">(((G38-F38)/2)+F38)</f>
         <v>0.33506944444444442</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" ref="I38:I45" si="15">H38-F38</f>
+        <f t="shared" ref="I38:I45" si="30">H38-F38</f>
         <v>1.7361111111111049E-3</v>
       </c>
       <c r="J38" s="2">
-        <f>((E38-D38)/2)+D38</f>
+        <f t="shared" si="27"/>
         <v>3.5</v>
       </c>
       <c r="K38" s="2">
-        <f>E38-J38</f>
+        <f t="shared" si="28"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1853,27 +1868,27 @@
         <v>5</v>
       </c>
       <c r="F39" s="1">
-        <f>((B39+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.3298611111111111</v>
       </c>
       <c r="G39" s="1">
-        <f>((C39+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.33159722222222221</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>1.7361111111111049E-3</v>
       </c>
       <c r="J39" s="2">
-        <f>((E39-D39)/2)+D39</f>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="K39" s="2">
-        <f>E39-J39</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
     </row>
@@ -1894,27 +1909,27 @@
         <v>-1</v>
       </c>
       <c r="F40" s="1">
-        <f>((B40+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.75</v>
       </c>
       <c r="G40" s="1">
-        <f>((C40+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.76388888888888884</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.75694444444444442</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J40" s="2">
-        <f>((E40-D40)/2)+D40</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K40" s="2">
-        <f>E40-J40</f>
+        <f t="shared" si="28"/>
         <v>-1</v>
       </c>
     </row>
@@ -1935,27 +1950,27 @@
         <v>30</v>
       </c>
       <c r="F41" s="1">
-        <f>((B41+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.76736111111111116</v>
       </c>
       <c r="G41" s="1">
-        <f>((C41+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.77083333333333337</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.76909722222222232</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>1.7361111111111605E-3</v>
       </c>
       <c r="J41" s="2">
-        <f>((E41-D41)/2)+D41</f>
+        <f t="shared" si="27"/>
         <v>30</v>
       </c>
       <c r="K41" s="2">
-        <f>E41-J41</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -1976,27 +1991,27 @@
         <v>15</v>
       </c>
       <c r="F42" s="1">
-        <f>((B42+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G42" s="1">
-        <f>((C42+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.79861111111111116</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.79513888888888884</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="J42" s="2">
-        <f>((E42-D42)/2)+D42</f>
+        <f t="shared" si="27"/>
         <v>11.5</v>
       </c>
       <c r="K42" s="2">
-        <f>E42-J42</f>
+        <f t="shared" si="28"/>
         <v>3.5</v>
       </c>
     </row>
@@ -2017,27 +2032,27 @@
         <v>30</v>
       </c>
       <c r="F43" s="1">
-        <f>((B43+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G43" s="1">
-        <f>((C43+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.85416666666666663</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.84375</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J43" s="2">
-        <f>((E43-D43)/2)+D43</f>
+        <f t="shared" si="27"/>
         <v>25</v>
       </c>
       <c r="K43" s="2">
-        <f>E43-J43</f>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
     </row>
@@ -2058,27 +2073,27 @@
         <v>-1</v>
       </c>
       <c r="F44" s="1">
-        <f>((B44+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.88194444444444453</v>
       </c>
       <c r="G44" s="1">
-        <f>((C44+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.89583333333333337</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.88888888888888895</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J44" s="2">
-        <f>((E44-D44)/2)+D44</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K44" s="2">
-        <f>E44-J44</f>
+        <f t="shared" si="28"/>
         <v>-1</v>
       </c>
     </row>
@@ -2099,27 +2114,27 @@
         <v>-1</v>
       </c>
       <c r="F45" s="1">
-        <f>((B45+360)/60)/24</f>
+        <f t="shared" si="23"/>
         <v>0.95833333333333337</v>
       </c>
       <c r="G45" s="1">
-        <f>((C45+360)/60)/24</f>
+        <f t="shared" si="24"/>
         <v>0.97916666666666663</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>0.96875</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="30"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J45" s="2">
-        <f>((E45-D45)/2)+D45</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K45" s="2">
-        <f>E45-J45</f>
+        <f t="shared" si="28"/>
         <v>-1</v>
       </c>
     </row>
@@ -2155,11 +2170,11 @@
         <v>160</v>
       </c>
       <c r="F48" s="1">
-        <f>((B48+360)/60)/24</f>
+        <f t="shared" ref="F48:F58" si="31">((B48+360)/60)/24</f>
         <v>0.25</v>
       </c>
       <c r="G48" s="1">
-        <f>((C48+360)/60)/24</f>
+        <f t="shared" ref="G48:G58" si="32">((C48+360)/60)/24</f>
         <v>0.2638888888888889</v>
       </c>
       <c r="H48" s="1">
@@ -2171,11 +2186,11 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="J48" s="2">
-        <f>((E48-D48)/2)+D48</f>
+        <f t="shared" ref="J48:J58" si="33">((E48-D48)/2)+D48</f>
         <v>145</v>
       </c>
       <c r="K48" s="2">
-        <f>E48-J48</f>
+        <f t="shared" ref="K48:K58" si="34">E48-J48</f>
         <v>15</v>
       </c>
       <c r="L48" s="2"/>
@@ -2199,27 +2214,27 @@
         <v>5</v>
       </c>
       <c r="F49" s="1">
-        <f>((B49+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.2673611111111111</v>
       </c>
       <c r="G49" s="1">
-        <f>((C49+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" ref="H49:H58" si="16">(((G49-F49)/2)+F49)</f>
+        <f t="shared" ref="H49:H58" si="35">(((G49-F49)/2)+F49)</f>
         <v>0.27256944444444442</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" ref="I49:I58" si="17">H49-F49</f>
+        <f t="shared" ref="I49:I58" si="36">H49-F49</f>
         <v>5.2083333333333148E-3</v>
       </c>
       <c r="J49" s="2">
-        <f>((E49-D49)/2)+D49</f>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
       <c r="K49" s="2">
-        <f>E49-J49</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="M49" s="1"/>
@@ -2242,27 +2257,27 @@
         <v>10</v>
       </c>
       <c r="F50" s="1">
-        <f>((B50+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.29166666666666669</v>
       </c>
       <c r="G50" s="1">
-        <f>((C50+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.3125</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.30208333333333337</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="J50" s="2">
-        <f>((E50-D50)/2)+D50</f>
+        <f t="shared" si="33"/>
         <v>9</v>
       </c>
       <c r="K50" s="2">
-        <f>E50-J50</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="M50" s="1"/>
@@ -2285,27 +2300,27 @@
         <v>-1</v>
       </c>
       <c r="F51" s="1">
-        <f>((B51+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.3888888888888889</v>
       </c>
       <c r="G51" s="1">
-        <f>((C51+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.40972222222222227</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.39930555555555558</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="J51" s="2">
-        <f>((E51-D51)/2)+D51</f>
+        <f t="shared" si="33"/>
         <v>-1</v>
       </c>
       <c r="K51" s="2">
-        <f>E51-J51</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M51" s="1"/>
@@ -2328,27 +2343,27 @@
         <v>20</v>
       </c>
       <c r="F52" s="1">
-        <f>((B52+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.44791666666666669</v>
       </c>
       <c r="G52" s="1">
-        <f>((C52+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.4861111111111111</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.4670138888888889</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.909722222222221E-2</v>
       </c>
       <c r="J52" s="2">
-        <f>((E52-D52)/2)+D52</f>
+        <f t="shared" si="33"/>
         <v>15</v>
       </c>
       <c r="K52" s="2">
-        <f>E52-J52</f>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="M52" s="1"/>
@@ -2371,27 +2386,27 @@
         <v>30</v>
       </c>
       <c r="F53" s="1">
-        <f>((B53+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G53" s="1">
-        <f>((C53+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.51041666666666674</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="J53" s="2">
-        <f>((E53-D53)/2)+D53</f>
+        <f t="shared" si="33"/>
         <v>27.5</v>
       </c>
       <c r="K53" s="2">
-        <f>E53-J53</f>
+        <f t="shared" si="34"/>
         <v>2.5</v>
       </c>
       <c r="M53" s="1"/>
@@ -2414,27 +2429,27 @@
         <v>30</v>
       </c>
       <c r="F54" s="1">
-        <f>((B54+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G54" s="1">
-        <f>((C54+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.51041666666666674</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="J54" s="2">
-        <f>((E54-D54)/2)+D54</f>
+        <f t="shared" si="33"/>
         <v>27.5</v>
       </c>
       <c r="K54" s="2">
-        <f>E54-J54</f>
+        <f t="shared" si="34"/>
         <v>2.5</v>
       </c>
       <c r="M54" s="1"/>
@@ -2457,27 +2472,27 @@
         <v>30</v>
       </c>
       <c r="F55" s="1">
-        <f>((B55+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G55" s="1">
-        <f>((C55+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.51041666666666674</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="J55" s="2">
-        <f>((E55-D55)/2)+D55</f>
+        <f t="shared" si="33"/>
         <v>27.5</v>
       </c>
       <c r="K55" s="2">
-        <f>E55-J55</f>
+        <f t="shared" si="34"/>
         <v>2.5</v>
       </c>
       <c r="M55" s="1"/>
@@ -2500,27 +2515,27 @@
         <v>60</v>
       </c>
       <c r="F56" s="1">
-        <f>((B56+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="G56" s="1">
-        <f>((C56+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.8125</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.80208333333333326</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="J56" s="2">
-        <f>((E56-D56)/2)+D56</f>
+        <f t="shared" si="33"/>
         <v>60</v>
       </c>
       <c r="K56" s="2">
-        <f>E56-J56</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M56" s="1"/>
@@ -2543,27 +2558,27 @@
         <v>-1</v>
       </c>
       <c r="F57" s="1">
-        <f>((B57+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.85416666666666663</v>
       </c>
       <c r="G57" s="1">
-        <f>((C57+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.89583333333333337</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.875</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="J57" s="2">
-        <f>((E57-D57)/2)+D57</f>
+        <f t="shared" si="33"/>
         <v>-1</v>
       </c>
       <c r="K57" s="2">
-        <f>E57-J57</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M57" s="1"/>
@@ -2586,31 +2601,1178 @@
         <v>30</v>
       </c>
       <c r="F58" s="1">
-        <f>((B58+360)/60)/24</f>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G58" s="1">
-        <f>((C58+360)/60)/24</f>
+        <f t="shared" si="32"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="35"/>
         <v>0.51041666666666674</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="36"/>
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="J58" s="2">
-        <f>((E58-D58)/2)+D58</f>
+        <f t="shared" si="33"/>
         <v>27.5</v>
       </c>
       <c r="K58" s="2">
-        <f>E58-J58</f>
+        <f t="shared" si="34"/>
         <v>2.5</v>
       </c>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>90</v>
+      </c>
+      <c r="C60">
+        <v>110</v>
+      </c>
+      <c r="D60">
+        <v>270</v>
+      </c>
+      <c r="E60">
+        <v>300</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" ref="F60" si="37">((B60+360)/60)/24</f>
+        <v>0.3125</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" ref="G60" si="38">((C60+360)/60)/24</f>
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" ref="H60" si="39">(((G60-F60)/2)+F60)</f>
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="I60" s="1">
+        <f t="shared" ref="I60" si="40">H60-F60</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" ref="J60" si="41">((E60-D60)/2)+D60</f>
+        <v>285</v>
+      </c>
+      <c r="K60" s="2">
+        <f t="shared" ref="K60" si="42">E60-J60</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>150</v>
+      </c>
+      <c r="C61">
+        <v>160</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" ref="F61:F67" si="43">((B61+360)/60)/24</f>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" ref="G61:G67" si="44">((C61+360)/60)/24</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" ref="H61:H67" si="45">(((G61-F61)/2)+F61)</f>
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="I61" s="1">
+        <f t="shared" ref="I61:I67" si="46">H61-F61</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" ref="J61:J67" si="47">((E61-D61)/2)+D61</f>
+        <v>2</v>
+      </c>
+      <c r="K61" s="2">
+        <f t="shared" ref="K61:K67" si="48">E61-J61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>115</v>
+      </c>
+      <c r="C62">
+        <v>140</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>5</v>
+      </c>
+      <c r="F62" s="1">
+        <f t="shared" si="43"/>
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="44"/>
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H62" s="1">
+        <f t="shared" si="45"/>
+        <v>0.33854166666666669</v>
+      </c>
+      <c r="I62" s="1">
+        <f t="shared" si="46"/>
+        <v>8.6805555555555802E-3</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" si="47"/>
+        <v>5</v>
+      </c>
+      <c r="K62" s="2">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63">
+        <v>170</v>
+      </c>
+      <c r="C63">
+        <v>180</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>10</v>
+      </c>
+      <c r="F63" s="1">
+        <f t="shared" si="43"/>
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="44"/>
+        <v>0.375</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" si="45"/>
+        <v>0.37152777777777779</v>
+      </c>
+      <c r="I63" s="1">
+        <f t="shared" si="46"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" si="47"/>
+        <v>7.5</v>
+      </c>
+      <c r="K63" s="2">
+        <f t="shared" si="48"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64">
+        <v>120</v>
+      </c>
+      <c r="C64">
+        <v>350</v>
+      </c>
+      <c r="E64">
+        <v>-1</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="43"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="44"/>
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="45"/>
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="I64" s="1">
+        <f t="shared" si="46"/>
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="47"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K64" s="2">
+        <f t="shared" si="48"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>810</v>
+      </c>
+      <c r="C65">
+        <v>840</v>
+      </c>
+      <c r="E65">
+        <v>-1</v>
+      </c>
+      <c r="F65" s="1">
+        <f t="shared" si="43"/>
+        <v>0.8125</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="44"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="45"/>
+        <v>0.82291666666666674</v>
+      </c>
+      <c r="I65" s="1">
+        <f t="shared" si="46"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="47"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K65" s="2">
+        <f t="shared" si="48"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>900</v>
+      </c>
+      <c r="C66">
+        <v>930</v>
+      </c>
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>120</v>
+      </c>
+      <c r="F66" s="1">
+        <f t="shared" si="43"/>
+        <v>0.875</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="44"/>
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" si="45"/>
+        <v>0.88541666666666674</v>
+      </c>
+      <c r="I66" s="1">
+        <f t="shared" si="46"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" si="47"/>
+        <v>110</v>
+      </c>
+      <c r="K66" s="2">
+        <f t="shared" si="48"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>1020</v>
+      </c>
+      <c r="C67">
+        <v>1080</v>
+      </c>
+      <c r="E67">
+        <v>-1</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" si="43"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="H67" s="1">
+        <f t="shared" si="45"/>
+        <v>0.97916666666666674</v>
+      </c>
+      <c r="I67" s="1">
+        <f t="shared" si="46"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" si="47"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K67" s="2">
+        <f t="shared" si="48"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>60</v>
+      </c>
+      <c r="C69">
+        <v>80</v>
+      </c>
+      <c r="E69">
+        <v>-1</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" ref="F69" si="49">((B69+360)/60)/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" ref="G69" si="50">((C69+360)/60)/24</f>
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="H69" s="1">
+        <f t="shared" ref="H69" si="51">(((G69-F69)/2)+F69)</f>
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="I69" s="1">
+        <f t="shared" ref="I69" si="52">H69-F69</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" ref="J69" si="53">((E69-D69)/2)+D69</f>
+        <v>-0.5</v>
+      </c>
+      <c r="K69" s="2">
+        <f t="shared" ref="K69" si="54">E69-J69</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>120</v>
+      </c>
+      <c r="C70">
+        <v>240</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>10</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" ref="F70:F78" si="55">((B70+360)/60)/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" ref="G70:G78" si="56">((C70+360)/60)/24</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H70" s="1">
+        <f t="shared" ref="H70:H78" si="57">(((G70-F70)/2)+F70)</f>
+        <v>0.375</v>
+      </c>
+      <c r="I70" s="1">
+        <f t="shared" ref="I70:I78" si="58">H70-F70</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" ref="J70:J78" si="59">((E70-D70)/2)+D70</f>
+        <v>9</v>
+      </c>
+      <c r="K70" s="2">
+        <f t="shared" ref="K70:K78" si="60">E70-J70</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71">
+        <v>60</v>
+      </c>
+      <c r="C71">
+        <v>90</v>
+      </c>
+      <c r="D71">
+        <v>540</v>
+      </c>
+      <c r="E71">
+        <v>600</v>
+      </c>
+      <c r="F71" s="1">
+        <f t="shared" si="55"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="56"/>
+        <v>0.3125</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" si="57"/>
+        <v>0.30208333333333337</v>
+      </c>
+      <c r="I71" s="1">
+        <f t="shared" si="58"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="J71" s="2">
+        <f t="shared" si="59"/>
+        <v>570</v>
+      </c>
+      <c r="K71" s="2">
+        <f t="shared" si="60"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>330</v>
+      </c>
+      <c r="C72">
+        <v>360</v>
+      </c>
+      <c r="D72">
+        <v>8</v>
+      </c>
+      <c r="E72">
+        <v>15</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="55"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="56"/>
+        <v>0.5</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="57"/>
+        <v>0.48958333333333337</v>
+      </c>
+      <c r="I72" s="1">
+        <f t="shared" si="58"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="J72" s="2">
+        <f t="shared" si="59"/>
+        <v>11.5</v>
+      </c>
+      <c r="K72" s="2">
+        <f t="shared" si="60"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73">
+        <v>90</v>
+      </c>
+      <c r="C73">
+        <v>1010</v>
+      </c>
+      <c r="E73">
+        <v>-1</v>
+      </c>
+      <c r="F73" s="1">
+        <f t="shared" si="55"/>
+        <v>0.3125</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="56"/>
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="57"/>
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="I73" s="1">
+        <f t="shared" si="58"/>
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="J73" s="2">
+        <f t="shared" si="59"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K73" s="2">
+        <f t="shared" si="60"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74">
+        <v>390</v>
+      </c>
+      <c r="C74">
+        <v>420</v>
+      </c>
+      <c r="D74">
+        <v>15</v>
+      </c>
+      <c r="E74">
+        <v>20</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="55"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="56"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="57"/>
+        <v>0.53125</v>
+      </c>
+      <c r="I74" s="1">
+        <f t="shared" si="58"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J74" s="2">
+        <f t="shared" si="59"/>
+        <v>17.5</v>
+      </c>
+      <c r="K74" s="2">
+        <f t="shared" si="60"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>390</v>
+      </c>
+      <c r="C75">
+        <v>420</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
+      </c>
+      <c r="E75">
+        <v>5</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="55"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="56"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="57"/>
+        <v>0.53125</v>
+      </c>
+      <c r="I75" s="1">
+        <f t="shared" si="58"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J75" s="2">
+        <f t="shared" si="59"/>
+        <v>5</v>
+      </c>
+      <c r="K75" s="2">
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>720</v>
+      </c>
+      <c r="C76">
+        <v>780</v>
+      </c>
+      <c r="E76">
+        <v>-1</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="55"/>
+        <v>0.75</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="56"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="57"/>
+        <v>0.77083333333333326</v>
+      </c>
+      <c r="I76" s="1">
+        <f t="shared" si="58"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="J76" s="2">
+        <f t="shared" si="59"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K76" s="2">
+        <f t="shared" si="60"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77">
+        <v>780</v>
+      </c>
+      <c r="C77">
+        <v>810</v>
+      </c>
+      <c r="D77">
+        <v>180</v>
+      </c>
+      <c r="E77">
+        <v>200</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="55"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="56"/>
+        <v>0.8125</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="57"/>
+        <v>0.80208333333333326</v>
+      </c>
+      <c r="I77" s="1">
+        <f t="shared" si="58"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J77" s="2">
+        <f t="shared" si="59"/>
+        <v>190</v>
+      </c>
+      <c r="K77" s="2">
+        <f t="shared" si="60"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>960</v>
+      </c>
+      <c r="C78">
+        <v>1020</v>
+      </c>
+      <c r="E78">
+        <v>-1</v>
+      </c>
+      <c r="F78" s="1">
+        <f t="shared" si="55"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="56"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="H78" s="1">
+        <f t="shared" si="57"/>
+        <v>0.9375</v>
+      </c>
+      <c r="I78" s="1">
+        <f t="shared" si="58"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="J78" s="2">
+        <f t="shared" si="59"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K78" s="2">
+        <f t="shared" si="60"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>110</v>
+      </c>
+      <c r="D80">
+        <v>170</v>
+      </c>
+      <c r="E80">
+        <v>190</v>
+      </c>
+      <c r="F80" s="1">
+        <f t="shared" ref="F80" si="61">((B80+360)/60)/24</f>
+        <v>0.3125</v>
+      </c>
+      <c r="G80" s="1">
+        <f t="shared" ref="G80" si="62">((C80+360)/60)/24</f>
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="H80" s="1">
+        <f t="shared" ref="H80" si="63">(((G80-F80)/2)+F80)</f>
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="I80" s="1">
+        <f t="shared" ref="I80" si="64">H80-F80</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="J80" s="3">
+        <f t="shared" ref="J80" si="65">((E80-D80)/2)+D80</f>
+        <v>180</v>
+      </c>
+      <c r="K80" s="2">
+        <f t="shared" ref="K80" si="66">E80-J80</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81">
+        <v>110</v>
+      </c>
+      <c r="C81">
+        <v>120</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81" s="1">
+        <f t="shared" ref="F81:F90" si="67">((B81+360)/60)/24</f>
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" ref="G81:G90" si="68">((C81+360)/60)/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" ref="H81:H90" si="69">(((G81-F81)/2)+F81)</f>
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="I81" s="1">
+        <f t="shared" ref="I81:I90" si="70">H81-F81</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="J81" s="2">
+        <f t="shared" ref="J81:J90" si="71">((E81-D81)/2)+D81</f>
+        <v>3.5</v>
+      </c>
+      <c r="K81" s="2">
+        <f t="shared" ref="K81:K90" si="72">E81-J81</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82">
+        <v>110</v>
+      </c>
+      <c r="C82">
+        <v>225</v>
+      </c>
+      <c r="D82">
+        <v>25</v>
+      </c>
+      <c r="E82">
+        <v>30</v>
+      </c>
+      <c r="F82" s="1">
+        <f t="shared" si="67"/>
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="68"/>
+        <v>0.40625</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="69"/>
+        <v>0.36631944444444442</v>
+      </c>
+      <c r="I82" s="1">
+        <f t="shared" si="70"/>
+        <v>3.9930555555555525E-2</v>
+      </c>
+      <c r="J82" s="2">
+        <f t="shared" si="71"/>
+        <v>27.5</v>
+      </c>
+      <c r="K82" s="2">
+        <f t="shared" si="72"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>340</v>
+      </c>
+      <c r="C83">
+        <v>360</v>
+      </c>
+      <c r="E83">
+        <v>-1</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" si="67"/>
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="68"/>
+        <v>0.5</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="69"/>
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="I83" s="1">
+        <f t="shared" si="70"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="J83" s="2">
+        <f t="shared" si="71"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K83" s="2">
+        <f t="shared" si="72"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84">
+        <v>390</v>
+      </c>
+      <c r="C84">
+        <v>420</v>
+      </c>
+      <c r="D84">
+        <v>10</v>
+      </c>
+      <c r="E84">
+        <v>15</v>
+      </c>
+      <c r="F84" s="1">
+        <f t="shared" si="67"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="68"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="69"/>
+        <v>0.53125</v>
+      </c>
+      <c r="I84" s="1">
+        <f t="shared" si="70"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J84" s="2">
+        <f t="shared" si="71"/>
+        <v>12.5</v>
+      </c>
+      <c r="K84" s="2">
+        <f t="shared" si="72"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85">
+        <v>390</v>
+      </c>
+      <c r="C85">
+        <v>420</v>
+      </c>
+      <c r="D85">
+        <v>25</v>
+      </c>
+      <c r="E85">
+        <v>30</v>
+      </c>
+      <c r="F85" s="1">
+        <f t="shared" si="67"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="68"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="69"/>
+        <v>0.53125</v>
+      </c>
+      <c r="I85" s="1">
+        <f t="shared" si="70"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J85" s="2">
+        <f t="shared" si="71"/>
+        <v>27.5</v>
+      </c>
+      <c r="K85" s="2">
+        <f t="shared" si="72"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86">
+        <v>390</v>
+      </c>
+      <c r="C86">
+        <v>420</v>
+      </c>
+      <c r="D86">
+        <v>15</v>
+      </c>
+      <c r="E86">
+        <v>20</v>
+      </c>
+      <c r="F86" s="1">
+        <f t="shared" si="67"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="68"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="69"/>
+        <v>0.53125</v>
+      </c>
+      <c r="I86" s="1">
+        <f t="shared" si="70"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="J86" s="2">
+        <f t="shared" si="71"/>
+        <v>17.5</v>
+      </c>
+      <c r="K86" s="2">
+        <f t="shared" si="72"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <v>110</v>
+      </c>
+      <c r="C87">
+        <v>225</v>
+      </c>
+      <c r="D87">
+        <v>25</v>
+      </c>
+      <c r="E87">
+        <v>30</v>
+      </c>
+      <c r="F87" s="1">
+        <f t="shared" si="67"/>
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="68"/>
+        <v>0.40625</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="69"/>
+        <v>0.36631944444444442</v>
+      </c>
+      <c r="I87" s="1">
+        <f t="shared" si="70"/>
+        <v>3.9930555555555525E-2</v>
+      </c>
+      <c r="J87" s="2">
+        <f t="shared" si="71"/>
+        <v>27.5</v>
+      </c>
+      <c r="K87" s="2">
+        <f t="shared" si="72"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>18</v>
+      </c>
+      <c r="B88">
+        <v>900</v>
+      </c>
+      <c r="C88">
+        <v>930</v>
+      </c>
+      <c r="D88">
+        <v>100</v>
+      </c>
+      <c r="E88">
+        <v>120</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="67"/>
+        <v>0.875</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="68"/>
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="69"/>
+        <v>0.88541666666666674</v>
+      </c>
+      <c r="I88" s="1">
+        <f t="shared" si="70"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="J88" s="2">
+        <f t="shared" si="71"/>
+        <v>110</v>
+      </c>
+      <c r="K88" s="2">
+        <f t="shared" si="72"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89">
+        <v>1070</v>
+      </c>
+      <c r="C89">
+        <v>1080</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+      <c r="E89">
+        <v>-1</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" si="67"/>
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="68"/>
+        <v>1</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="69"/>
+        <v>0.99652777777777768</v>
+      </c>
+      <c r="I89" s="1">
+        <f t="shared" si="70"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="J89" s="2">
+        <f t="shared" si="71"/>
+        <v>-1</v>
+      </c>
+      <c r="K89" s="2">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>